<commit_message>
restructured, quick-start its own html page, shorter overview, and a lot more written
</commit_message>
<xml_diff>
--- a/Commutator BoM.xlsx
+++ b/Commutator BoM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cshor\Desktop\open ephys\commutator\commutator-docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E871A607-A81E-473E-BD69-A78D24A2F8CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B53C477-0ECC-4D84-835D-DE1382B77E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="30" windowWidth="16125" windowHeight="15585" xr2:uid="{2DB1BB45-703E-46D4-A2C0-E7B37BDB487D}"/>
+    <workbookView xWindow="2640" yWindow="1230" windowWidth="21600" windowHeight="11295" xr2:uid="{2DB1BB45-703E-46D4-A2C0-E7B37BDB487D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -145,7 +145,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -189,15 +189,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -259,17 +250,6 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -327,52 +307,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -691,7 +670,7 @@
   <dimension ref="C3:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -702,231 +681,230 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
     </row>
     <row r="6" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="11">
         <v>1</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="28">
+      <c r="F6" s="17">
         <v>92.57</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="13">
         <v>1</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="29">
+      <c r="F7" s="18">
         <v>350.99</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="9" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="24"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="23"/>
     </row>
     <row r="9" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="11">
         <v>1</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="28">
+      <c r="F9" s="17">
         <v>28.75</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="9" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="20">
+      <c r="D10" s="12">
         <v>1</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="30">
+      <c r="F10" s="19">
         <v>20.25</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="G10" s="9" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C11" s="10"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="15"/>
+      <c r="C11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="12">
+        <v>1</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="12" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="6"/>
-    </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C14" s="16" t="s">
+      <c r="C12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="13">
+        <v>1</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="F13" s="3">
+        <v>492.56</v>
+      </c>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C15" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="18"/>
-    </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C15" s="25" t="s">
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="26"/>
+    </row>
+    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C16" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="26" t="s">
+      <c r="E16" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G15" s="27" t="s">
+      <c r="G16" s="16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C16" s="9" t="s">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C17" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="20">
+      <c r="D17" s="12">
         <v>1</v>
       </c>
-      <c r="E16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="G16" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="9" t="s">
+      <c r="E17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="20">
+      <c r="D18" s="12">
         <v>1</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="G17" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="20">
-        <v>1</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="G18" s="13" t="s">
+      <c r="E18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" s="10" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="21">
-        <v>1</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="G19" s="14" t="s">
-        <v>20</v>
-      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="C3:G3"/>
     <mergeCell ref="C5:G5"/>
     <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C15:G15"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G6" r:id="rId1" xr:uid="{F339D0DF-7109-44E4-A5F9-F550D6F0DB9C}"/>

</xml_diff>